<commit_message>
refactor to extract utils
</commit_message>
<xml_diff>
--- a/common-excel/src/test/resources/test.xlsx
+++ b/common-excel/src/test/resources/test.xlsx
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Product Mix" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="test_name">'Product Mix'!$D$3</definedName>
+  </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -389,7 +392,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>